<commit_message>
Some kaggle submissions after..
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Projects\PWProject\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Guilherme Teixeira\Documents\Transferir\FCT\Workspace\PW Project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="6825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14268" windowHeight="6828"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>Run</t>
   </si>
@@ -138,6 +138,36 @@
   </si>
   <si>
     <t>0.0581</t>
+  </si>
+  <si>
+    <t>0.0402</t>
+  </si>
+  <si>
+    <t>0.0806</t>
+  </si>
+  <si>
+    <t>0.0081</t>
+  </si>
+  <si>
+    <t>0.0129</t>
+  </si>
+  <si>
+    <t>0.0368</t>
+  </si>
+  <si>
+    <t>0.0839</t>
+  </si>
+  <si>
+    <t>0.0248</t>
+  </si>
+  <si>
+    <t>0.0710</t>
+  </si>
+  <si>
+    <t>0.0387</t>
+  </si>
+  <si>
+    <t>0.0164</t>
   </si>
 </sst>
 </file>
@@ -192,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -490,19 +520,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -636,17 +653,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -672,30 +678,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
@@ -709,40 +703,45 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,7 +760,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1057,141 +1056,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R16"/>
+  <dimension ref="A2:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="C19" sqref="C19:P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" customWidth="1"/>
+    <col min="13" max="13" width="6.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
-      <c r="C3" s="8" t="s">
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6"/>
+      <c r="C3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="6" t="s">
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="7"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="P3" s="53"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="16">
         <v>0</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="24" t="s">
+      <c r="I5" s="18"/>
+      <c r="J5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="27" t="s">
+      <c r="K5" s="21"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="29">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="25">
         <v>1</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="36"/>
-      <c r="L6" s="38"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="1"/>
       <c r="N6" s="5"/>
       <c r="O6" s="3" t="s">
@@ -1201,24 +1200,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="29">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="25">
         <v>2</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="38"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="38"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
       <c r="M7" s="1"/>
       <c r="N7" s="5"/>
       <c r="O7" s="3" t="s">
@@ -1227,27 +1226,27 @@
       <c r="P7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="34"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="29">
+      <c r="Q7" s="31"/>
+      <c r="R7" s="30"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="25">
         <v>3</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="38"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="27" t="s">
         <v>24</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="38"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
       <c r="M8" s="1"/>
       <c r="N8" s="5"/>
       <c r="O8" s="3" t="s">
@@ -1256,26 +1255,26 @@
       <c r="P8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="33"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="29">
+      <c r="Q8" s="29"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="25">
         <v>4</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="38"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="27" t="s">
         <v>27</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="38"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="1"/>
       <c r="N9" s="5"/>
       <c r="O9" s="3" t="s">
@@ -1285,24 +1284,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="29">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="25">
         <v>5</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="27" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="38"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
       <c r="M10" s="1"/>
       <c r="N10" s="5"/>
       <c r="O10" s="3" t="s">
@@ -1312,24 +1311,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="29">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="25">
         <v>6</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="27" t="s">
         <v>24</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="32" t="s">
+      <c r="J11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="38"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
       <c r="M11" s="1"/>
       <c r="N11" s="5"/>
       <c r="O11" s="3" t="s">
@@ -1339,121 +1338,335 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="42">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="35">
         <v>7</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="46" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="47" t="s">
+      <c r="I12" s="37"/>
+      <c r="J12" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="48"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="50" t="s">
+      <c r="K12" s="41"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="P12" s="51" t="s">
+      <c r="P12" s="44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
-      <c r="B13" s="59">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="50"/>
+      <c r="B13" s="48">
         <v>8</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="31" t="s">
+      <c r="E13" s="33"/>
+      <c r="F13" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="31" t="s">
+      <c r="G13" s="33"/>
+      <c r="H13" s="27" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="38"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
       <c r="M13" s="1"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="50" t="s">
+      <c r="O13" s="43" t="s">
         <v>36</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
-      <c r="B14" s="60">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="50"/>
+      <c r="B14" s="49">
         <v>9</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="53"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="46"/>
+      <c r="L14" s="33"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="59">
+      <c r="N14" s="24"/>
+      <c r="O14" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="50"/>
+      <c r="B15" s="48">
         <v>10</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="1"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="33"/>
+      <c r="H15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="33"/>
+      <c r="J15" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
       <c r="M15" s="1"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11">
+      <c r="O15" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="7">
         <v>11</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="13"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="21"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="7">
+        <v>12</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="32"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="7">
+        <v>13</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="7">
+        <v>14</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+    </row>
+    <row r="20" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="7">
+        <v>15</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+    </row>
+    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="7">
+        <v>16</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+    </row>
+    <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="7">
+        <v>17</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+    </row>
+    <row r="23" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="7">
+        <v>18</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+    </row>
+    <row r="24" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="7">
+        <v>19</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+    </row>
+    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="7">
+        <v>20</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Better results with different analyzers
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Guilherme Teixeira\Documents\Transferir\FCT\Workspace\PW Project\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Projects\PWProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14268" windowHeight="6828"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="6825"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>Run</t>
   </si>
@@ -168,13 +168,19 @@
   </si>
   <si>
     <t>0.0164</t>
+  </si>
+  <si>
+    <t>Offline Evaluation</t>
+  </si>
+  <si>
+    <t>Kaggle Evaluation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +195,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,8 +233,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -507,19 +531,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -670,6 +681,115 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -678,58 +798,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,6 +842,64 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,7 +918,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1056,617 +1214,631 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R25"/>
+  <dimension ref="A2:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:P25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" customWidth="1"/>
-    <col min="13" max="13" width="6.88671875" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6"/>
-      <c r="C3" s="51" t="s">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="53"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="P3" s="33"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="16">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="84">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="20" t="s">
+      <c r="I5" s="74"/>
+      <c r="J5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="23" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="65" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="85">
         <v>1</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="27" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="28" t="s">
+      <c r="I6" s="73"/>
+      <c r="J6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="3" t="s">
+      <c r="K6" s="76"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="67" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="85">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="27" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="28" t="s">
+      <c r="I7" s="73"/>
+      <c r="J7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="3" t="s">
+      <c r="K7" s="76"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="30"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="25">
+      <c r="Q7" s="19"/>
+      <c r="R7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="85">
         <v>3</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="27" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="28" t="s">
+      <c r="I8" s="73"/>
+      <c r="J8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="3" t="s">
+      <c r="K8" s="76"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="29"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="25">
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="85">
         <v>4</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="27" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="28" t="s">
+      <c r="I9" s="73"/>
+      <c r="J9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="3" t="s">
+      <c r="K9" s="76"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="67" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="85">
         <v>5</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="27" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="28" t="s">
+      <c r="I10" s="73"/>
+      <c r="J10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="3" t="s">
+      <c r="K10" s="76"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="67" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="85">
         <v>6</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="27" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="28" t="s">
+      <c r="I11" s="73"/>
+      <c r="J11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="3" t="s">
+      <c r="K11" s="76"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="P11" s="67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="86">
         <v>7</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="39" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="40" t="s">
+      <c r="I12" s="80"/>
+      <c r="J12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="41"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="43" t="s">
+      <c r="K12" s="77"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="P12" s="44" t="s">
+      <c r="P12" s="70" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="48">
+      <c r="R12" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="51"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="87">
         <v>8</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="27" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="27" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="28" t="s">
+      <c r="I13" s="73"/>
+      <c r="J13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="43" t="s">
+      <c r="K13" s="76"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="P13" s="67" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="49">
+      <c r="R13" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S13" s="52"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="88">
         <v>9</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="27" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="28" t="s">
+      <c r="G14" s="21"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="46"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="47" t="s">
+      <c r="K14" s="78"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="P14" s="67" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="48">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="87">
         <v>10</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="27" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="27" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="28" t="s">
+      <c r="I15" s="21"/>
+      <c r="J15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="47" t="s">
+      <c r="K15" s="79"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="P15" s="5" t="s">
+      <c r="P15" s="67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="89">
         <v>11</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="27" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="28" t="s">
+      <c r="G16" s="21"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="10" t="s">
+      <c r="K16" s="44"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="65" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="7">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="85">
         <v>12</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="27" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="28" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="32"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="10" t="s">
+      <c r="K17" s="76"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="70" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="7">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="86">
         <v>13</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="27" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="27" t="s">
+      <c r="G18" s="21"/>
+      <c r="H18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="28" t="s">
+      <c r="I18" s="73"/>
+      <c r="J18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="10" t="s">
+      <c r="K18" s="66"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="67" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="7">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="90">
         <v>14</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-    </row>
-    <row r="20" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="7">
+      <c r="C19" s="55"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="62">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="P19" s="63"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="23">
         <v>15</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-    </row>
-    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="7">
+      <c r="C20" s="20"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="41"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="23">
         <v>16</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-    </row>
-    <row r="22" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="7">
+      <c r="C21" s="20"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="42"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="23">
         <v>17</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-    </row>
-    <row r="23" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="7">
+      <c r="C22" s="29"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="43"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="23">
         <v>18</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-    </row>
-    <row r="24" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="7">
+      <c r="C23" s="20"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="23">
         <v>19</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-    </row>
-    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="7">
+      <c r="C24" s="20"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="50"/>
+    </row>
+    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="48">
         <v>20</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>